<commit_message>
Update Activity List, Gantt Chart, WBS
</commit_message>
<xml_diff>
--- a/Documentation/MCSPROJ/Activity List.xlsx
+++ b/Documentation/MCSPROJ/Activity List.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>Activity #</t>
   </si>
@@ -103,30 +103,6 @@
     <t>Design System</t>
   </si>
   <si>
-    <t>Design Database</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2;3 </t>
-  </si>
-  <si>
-    <t>7;8</t>
-  </si>
-  <si>
-    <t>7;8;9</t>
-  </si>
-  <si>
-    <t>7;8;9;10</t>
-  </si>
-  <si>
-    <t>3;7;8;9;10</t>
-  </si>
-  <si>
-    <t>3;7</t>
-  </si>
-  <si>
-    <t>3;5;7;8;9;10;12;18</t>
-  </si>
-  <si>
     <t>Plan for project features</t>
   </si>
   <si>
@@ -157,13 +133,52 @@
     <t>Gantt Chart</t>
   </si>
   <si>
-    <t xml:space="preserve">Working system </t>
-  </si>
-  <si>
-    <t>Database</t>
-  </si>
-  <si>
     <t>Prepared all project requirements</t>
+  </si>
+  <si>
+    <t>Business Rules</t>
+  </si>
+  <si>
+    <t>ERD</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Admin and User Interfaces</t>
+  </si>
+  <si>
+    <t>2;3</t>
+  </si>
+  <si>
+    <t>5;6</t>
+  </si>
+  <si>
+    <t>5;6;7</t>
+  </si>
+  <si>
+    <t>5;6;7;8</t>
+  </si>
+  <si>
+    <t>5;9</t>
+  </si>
+  <si>
+    <t>3;5;6;7;8</t>
+  </si>
+  <si>
+    <t>3;5;6;7;8;9;10;15</t>
+  </si>
+  <si>
+    <t>5;6;7;8;9;10</t>
+  </si>
+  <si>
+    <t>Develop Interfaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated system </t>
+  </si>
+  <si>
+    <t>Yii Framework</t>
   </si>
 </sst>
 </file>
@@ -515,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -592,11 +607,11 @@
       <c r="E3" s="4">
         <v>42538</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>27</v>
+      <c r="F3" s="1">
+        <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -615,11 +630,11 @@
       <c r="E4" s="4">
         <v>42541</v>
       </c>
-      <c r="F4" s="1">
-        <v>3</v>
+      <c r="F4" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -639,10 +654,10 @@
         <v>42546</v>
       </c>
       <c r="F5" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -662,10 +677,10 @@
         <v>42566</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -685,10 +700,10 @@
         <v>42586</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -708,208 +723,251 @@
         <v>42608</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E9" s="4">
-        <v>42608</v>
+        <v>42650</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="E10" s="4">
-        <v>42650</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>32</v>
+        <v>42548</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="E11" s="4">
-        <v>42548</v>
+        <v>42663</v>
+      </c>
+      <c r="F11" s="1">
+        <v>11</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D12" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E12" s="4">
-        <v>42636</v>
+        <v>42666</v>
+      </c>
+      <c r="F12" s="1">
+        <v>11</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E13" s="4">
-        <v>42663</v>
-      </c>
-      <c r="F13" s="1">
-        <v>14</v>
+        <v>42608</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" s="4">
-        <v>42666</v>
-      </c>
-      <c r="F14" s="1">
-        <v>14</v>
+        <v>42583</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="E15" s="4">
-        <v>42583</v>
+        <v>42628</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D16" s="1">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="E16" s="4">
-        <v>42628</v>
+        <v>42638</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E17" s="4">
         <v>42638</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>31</v>
+      <c r="F17" s="1">
+        <v>5</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>11</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1">
+        <v>60</v>
+      </c>
+      <c r="E18" s="4">
+        <v>42660</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="1">
+        <v>11</v>
+      </c>
+      <c r="E19" s="4">
+        <v>42636</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>